<commit_message>
Build fix excel writing code.
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TestDataGradeOne.xlsx
+++ b/src/main/resources/testData/TestDataGradeOne.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/QA-Automation/src/main/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143400E9-44AA-1A4F-8E6F-4BC382F13FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311BAAF1-C750-A44A-9CD5-F77E6B5F318C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="101">
   <si>
     <t>Password</t>
   </si>
@@ -296,15 +296,62 @@
   </si>
   <si>
     <t>event_7771002258369</t>
+  </si>
+  <si>
+    <t>Joe Customer</t>
+  </si>
+  <si>
+    <t>rcg+27585004@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585004</t>
+  </si>
+  <si>
+    <t>27585004</t>
+  </si>
+  <si>
+    <t>rcg+27585005@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585005</t>
+  </si>
+  <si>
+    <t>27585005</t>
+  </si>
+  <si>
+    <t>rcg+27585006@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585006</t>
+  </si>
+  <si>
+    <t>27585006</t>
+  </si>
+  <si>
+    <t>rcg+27585007@pcci.edu</t>
+  </si>
+  <si>
+    <t>rcg27585007</t>
+  </si>
+  <si>
+    <t>27585007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <numFmts count="0"/>
+  <fonts count="11">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -533,38 +580,39 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -850,16 +898,16 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.1953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -873,10 +921,18 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="8"/>
@@ -904,16 +960,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16">
@@ -970,10 +1026,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="25.83203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.83203125" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" width="25.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1192,9 +1248,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="34.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1711,13 +1767,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1879,9 +1935,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16">
@@ -1974,7 +2030,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16">
@@ -2011,8 +2067,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>